<commit_message>
SE-341 Validate the metabolomics data, not just the metadata.
SVN: 21590
</commit_message>
<xml_diff>
--- a/eu_basynthec/sourceTest/examples/Metabolomics-BadData.xlsx
+++ b/eu_basynthec/sourceTest/examples/Metabolomics-BadData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="1600" windowWidth="27520" windowHeight="12740" tabRatio="500"/>
+    <workbookView xWindow="860" yWindow="1600" windowWidth="27520" windowHeight="12740" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="openbis-metadata" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>One of mM, uM, RatioT1, or RatioCs</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -58,77 +58,74 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>HumanReadable</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Strain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value Unit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scale</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The openBIS experiment identifier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Strain Id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>One of Value, Mean, Median, Std, Var, Error, or Iqr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phosphate1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phosphate2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>strain1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>CompoundID</t>
-  </si>
-  <si>
-    <t>HumanReadable</t>
-  </si>
-  <si>
-    <t>Experiment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Strain</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Value Type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Value Unit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Scale</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The openBIS experiment identifier</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The Strain Id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>One of Value, Mean, Median, Std, Var, Error, or Iqr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CHEBI:15521</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CHEBI:18311</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>phosphate1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>phosphate2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>strain1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>foo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>foo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>foo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>foo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -554,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -578,22 +575,22 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -601,7 +598,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
@@ -612,7 +609,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>2</v>
@@ -620,21 +617,21 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>0</v>
@@ -642,10 +639,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>1</v>
@@ -669,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -682,10 +679,10 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
       </c>
       <c r="C1">
         <v>-703</v>
@@ -759,10 +756,10 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>9.5157063E-2</v>
@@ -836,10 +833,10 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>5.9749696999999997E-2</v>

</xml_diff>

<commit_message>
SE-341 Added handling of OD600 data.
SVN: 21605
</commit_message>
<xml_diff>
--- a/eu_basynthec/sourceTest/examples/Metabolomics-BadData.xlsx
+++ b/eu_basynthec/sourceTest/examples/Metabolomics-BadData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="1600" windowWidth="27520" windowHeight="12740" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="34320" windowHeight="22740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="openbis-metadata" sheetId="1" r:id="rId1"/>
@@ -22,115 +22,114 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
+    <t>One of Lin, Log2, Log10, or Ln</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>One of CE, ES, ME, CY, or NC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Property</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Timepoint Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>One of EX, IN, or SI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cell Location</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HumanReadable</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Strain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value Unit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scale</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The openBIS experiment identifier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Strain Id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>One of Value, Mean, Median, Std, Var, Error, or Iqr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phosphate1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phosphate2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompoundID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>foo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>One of mM, uM, RatioT1, or RatioCs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>One of Lin, Log2, Log10, or Ln</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>One of CE, ES, ME, CY, or NC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Property</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Timepoint Type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>One of EX, IN, or SI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cell Location</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HumanReadable</t>
-  </si>
-  <si>
-    <t>Experiment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Strain</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Value Type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Value Unit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Scale</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The openBIS experiment identifier</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The Strain Id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>One of Value, Mean, Median, Std, Var, Error, or Iqr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>phosphate1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>phosphate2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>strain1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>foo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>foo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>foo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>foo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>foo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CompoundID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>foo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -551,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -564,91 +563,92 @@
   <sheetData>
     <row r="1" spans="1:3" ht="20">
       <c r="A1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <colBreaks count="1" manualBreakCount="1">
@@ -666,7 +666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -679,10 +679,10 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1">
         <v>-703</v>
@@ -756,10 +756,10 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>9.5157063E-2</v>
@@ -833,10 +833,10 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>5.9749696999999997E-2</v>
@@ -909,6 +909,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
SP-29 BIS-28 Changed validator and handler to process the value unit in the metadata sheet.
SVN: 25287
</commit_message>
<xml_diff>
--- a/eu_basynthec/sourceTest/examples/Metabolomics-BadData.xlsx
+++ b/eu_basynthec/sourceTest/examples/Metabolomics-BadData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22220"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
   <si>
     <t>One of CE, ES, ME, CY, or NC</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -161,9 +161,6 @@
   <si>
     <t>foo</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>foo</t>
   </si>
 </sst>
 </file>
@@ -791,14 +788,14 @@
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>39</v>
+      <c r="B7" s="5">
+        <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="11">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -806,7 +803,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>24</v>

</xml_diff>